<commit_message>
new plots after new integral slurm
</commit_message>
<xml_diff>
--- a/assignment4/integral_plots.xlsx
+++ b/assignment4/integral_plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UTSA\Spring_2024\High Performance Computing\Week_5\HW_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B748DF47-14AA-4577-9E14-E258231E6CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BCA471-84E6-490A-B007-28BE251F5DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{99849A08-FDBF-461F-8D37-C3E8A5CBD3C4}"/>
   </bookViews>
@@ -266,16 +266,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>366.68039599999997</c:v>
+                  <c:v>358.37575099999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>380.08195899999998</c:v>
+                  <c:v>348.74953399999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>368.01578899999998</c:v>
+                  <c:v>360.318715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>367.127341</c:v>
+                  <c:v>369.46292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,16 +725,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15.389120999999999</c:v>
+                  <c:v>15.571873999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.322094</c:v>
+                  <c:v>15.549371000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.932916000000001</c:v>
+                  <c:v>15.671035</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.944799</c:v>
+                  <c:v>15.607931000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,13 +1192,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96474033380784585</c:v>
+                  <c:v>1.0276020927959146</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99637137035987333</c:v>
+                  <c:v>0.9946076517285537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99878258862774261</c:v>
+                  <c:v>0.96999111845919472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1648,16 +1648,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.006226</c:v>
+                  <c:v>13.190033</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1066490000000009</c:v>
+                  <c:v>8.6977700000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.419708</c:v>
+                  <c:v>6.5458550000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0363410000000002</c:v>
+                  <c:v>5.1077979999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2110,13 +2110,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0043745326193665</c:v>
+                  <c:v>1.0014471968030088</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0305502957359434</c:v>
+                  <c:v>0.9936723388085088</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0297308782807986</c:v>
+                  <c:v>0.99768982833150655</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2569,13 +2569,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.428212067907745</c:v>
+                  <c:v>1.5164844552109333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0259840478725826</c:v>
+                  <c:v>2.0150206504727035</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5824752533635031</c:v>
+                  <c:v>2.5823325432994806</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6783,13 +6783,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>366.68039599999997</v>
+        <v>358.37575099999998</v>
       </c>
       <c r="C2" s="1">
-        <v>15.389120999999999</v>
+        <v>15.571873999999999</v>
       </c>
       <c r="D2" s="1">
-        <v>13.006226</v>
+        <v>13.190033</v>
       </c>
       <c r="E2" s="1">
         <f>$B$2/B2</f>
@@ -6809,25 +6809,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>380.08195899999998</v>
+        <v>348.74953399999998</v>
       </c>
       <c r="C3" s="1">
-        <v>15.322094</v>
+        <v>15.549371000000001</v>
       </c>
       <c r="D3" s="1">
-        <v>9.1066490000000009</v>
+        <v>8.6977700000000002</v>
       </c>
       <c r="E3" s="1">
         <f>$B$2/B3</f>
-        <v>0.96474033380784585</v>
+        <v>1.0276020927959146</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F5" si="0">$C$2/C3</f>
-        <v>1.0043745326193665</v>
+        <v>1.0014471968030088</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G5" si="1">$D$2/D3</f>
-        <v>1.428212067907745</v>
+        <v>1.5164844552109333</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -6835,25 +6835,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>368.01578899999998</v>
+        <v>360.318715</v>
       </c>
       <c r="C4" s="1">
-        <v>14.932916000000001</v>
+        <v>15.671035</v>
       </c>
       <c r="D4" s="1">
-        <v>6.419708</v>
+        <v>6.5458550000000004</v>
       </c>
       <c r="E4" s="1">
         <f>$B$2/B4</f>
-        <v>0.99637137035987333</v>
+        <v>0.9946076517285537</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>1.0305502957359434</v>
+        <v>0.9936723388085088</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>2.0259840478725826</v>
+        <v>2.0150206504727035</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -6861,25 +6861,25 @@
         <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>367.127341</v>
+        <v>369.46292</v>
       </c>
       <c r="C5" s="1">
-        <v>14.944799</v>
+        <v>15.607931000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>5.0363410000000002</v>
+        <v>5.1077979999999998</v>
       </c>
       <c r="E5" s="1">
         <f>$B$2/B5</f>
-        <v>0.99878258862774261</v>
+        <v>0.96999111845919472</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>1.0297308782807986</v>
+        <v>0.99768982833150655</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>2.5824752533635031</v>
+        <v>2.5823325432994806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>